<commit_message>
minor changes on mapping of amazonia terms
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@73429 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/ICEMR terms.xlsx
+++ b/Load/src/ontology/ICEMR/ICEMR terms.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8856" uniqueCount="3312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8856" uniqueCount="3314">
   <si>
     <t>Term Ontology IRI</t>
   </si>
@@ -9992,14 +9992,27 @@
   <si>
     <t>http://purl.obolibrary.org/obo/ICEMR_10020177</t>
   </si>
+  <si>
+    <t>Hen</t>
+  </si>
+  <si>
+    <t>hen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -10232,251 +10245,252 @@
   </borders>
   <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -10844,9 +10858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103:B281"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G268" sqref="G268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17819,8 +17833,8 @@
       <c r="B267" t="s">
         <v>3299</v>
       </c>
-      <c r="C267" s="68" t="s">
-        <v>3135</v>
+      <c r="C267" s="101" t="s">
+        <v>3312</v>
       </c>
       <c r="D267" t="s">
         <v>1821</v>
@@ -17832,7 +17846,7 @@
         <v>3082</v>
       </c>
       <c r="G267" t="s">
-        <v>2903</v>
+        <v>3313</v>
       </c>
       <c r="H267" s="53" t="s">
         <v>1785</v>

</xml_diff>